<commit_message>
here is an update2
</commit_message>
<xml_diff>
--- a/src/main/java/com/spotify/resources/logincredentials.xlsx
+++ b/src/main/java/com/spotify/resources/logincredentials.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12495"/>
+    <workbookView windowWidth="28740" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
   <si>
     <t>testcaseid</t>
   </si>
@@ -31,7 +31,7 @@
     <t>expectedresult</t>
   </si>
   <si>
-    <t>Spotify_TC_1</t>
+    <t>Spotify_TC_3</t>
   </si>
   <si>
     <t>anandkushwaha064@gmail.com</t>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>firefox</t>
-  </si>
-  <si>
-    <t>Spotify_TC_3</t>
   </si>
   <si>
     <t>Spotify_TC_4</t>
@@ -144,10 +141,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -166,6 +163,81 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -174,18 +246,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -196,111 +298,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -311,181 +308,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -507,6 +504,17 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -514,16 +522,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -547,30 +570,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -579,26 +578,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -607,148 +604,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -756,60 +753,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="48" applyFont="true">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
     <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -938,7 +935,7 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -962,9 +959,9 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -988,7 +985,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -1041,7 +1038,7 @@
             <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill rotWithShape="true">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
@@ -1066,7 +1063,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="5400000" scaled="false"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1081,16 +1078,16 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="16.1428571428571" customWidth="1"/>
-    <col min="2" max="2" width="33.4285714285714" customWidth="1"/>
-    <col min="3" max="3" width="13.4285714285714" customWidth="1"/>
-    <col min="4" max="4" width="14.4285714285714" customWidth="1"/>
-    <col min="5" max="5" width="17.5714285714286" customWidth="1"/>
+    <col min="1" max="1" width="16.14" customWidth="true"/>
+    <col min="2" max="2" width="33.4266666666667" customWidth="true"/>
+    <col min="3" max="3" width="13.4266666666667" customWidth="true"/>
+    <col min="4" max="4" width="14.4266666666667" customWidth="true"/>
+    <col min="5" max="5" width="17.5733333333333" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1146,7 +1143,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>6</v>
@@ -1163,7 +1160,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1180,7 +1177,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
@@ -1197,7 +1194,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>6</v>
@@ -1214,7 +1211,7 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
@@ -1231,7 +1228,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
@@ -1248,7 +1245,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -1265,7 +1262,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>6</v>
@@ -1282,7 +1279,7 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>6</v>
@@ -1299,7 +1296,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>6</v>
@@ -1316,7 +1313,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
@@ -1333,7 +1330,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>6</v>
@@ -1350,7 +1347,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>6</v>
@@ -1367,7 +1364,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -1384,7 +1381,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>6</v>
@@ -1401,7 +1398,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>6</v>
@@ -1418,7 +1415,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -1435,7 +1432,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>6</v>
@@ -1452,7 +1449,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>6</v>
@@ -1469,7 +1466,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>6</v>
@@ -1486,7 +1483,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
@@ -1503,7 +1500,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>6</v>
@@ -1520,7 +1517,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>6</v>
@@ -1537,7 +1534,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>6</v>
@@ -1554,7 +1551,7 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>6</v>
@@ -1571,7 +1568,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>6</v>
@@ -1588,7 +1585,7 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -1605,7 +1602,7 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>6</v>
@@ -1622,7 +1619,7 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>6</v>
@@ -1639,7 +1636,7 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>6</v>
@@ -1656,7 +1653,6 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B7" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B13" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B18" r:id="rId1" display="anandkushwaha064@gmail.com"/>
@@ -1688,6 +1684,7 @@
     <hyperlink ref="B31" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B32" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B33" r:id="rId1" display="anandkushwaha064@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId1" display="anandkushwaha064@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
here is an update4
</commit_message>
<xml_diff>
--- a/src/main/java/com/spotify/resources/logincredentials.xlsx
+++ b/src/main/java/com/spotify/resources/logincredentials.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="46">
   <si>
     <t>testcaseid</t>
   </si>
@@ -134,6 +134,24 @@
   </si>
   <si>
     <t>Spotify_TC_32</t>
+  </si>
+  <si>
+    <t>Spotify_TC_33</t>
+  </si>
+  <si>
+    <t>anandkushwaha065@gmail.com</t>
+  </si>
+  <si>
+    <t>Spotify_TC_34</t>
+  </si>
+  <si>
+    <t>anandkushwaha066@gmail.com</t>
+  </si>
+  <si>
+    <t>Spotify_TC_35</t>
+  </si>
+  <si>
+    <t>anandkushwaha067@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -141,10 +159,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -163,6 +181,106 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -171,34 +289,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -208,96 +316,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -308,187 +326,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -499,6 +517,39 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -521,7 +572,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -541,35 +592,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -588,164 +617,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="7" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1075,10 +1093,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E38" sqref="C33:C36 E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="15.75" outlineLevelCol="4"/>
@@ -1648,6 +1666,57 @@
         <v>10</v>
       </c>
       <c r="E33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>40</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1685,6 +1754,9 @@
     <hyperlink ref="B32" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B33" r:id="rId1" display="anandkushwaha064@gmail.com"/>
     <hyperlink ref="B2" r:id="rId1" display="anandkushwaha064@gmail.com"/>
+    <hyperlink ref="B34" r:id="rId1" display="anandkushwaha065@gmail.com"/>
+    <hyperlink ref="B35" r:id="rId1" display="anandkushwaha066@gmail.com"/>
+    <hyperlink ref="B36" r:id="rId1" display="anandkushwaha067@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>